<commit_message>
first sheet for excel is working
</commit_message>
<xml_diff>
--- a/Reading_TTC_Excel/excel_files/TestOneTrain.xlsx
+++ b/Reading_TTC_Excel/excel_files/TestOneTrain.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Yonge-University" sheetId="1" r:id="rId1"/>
@@ -2063,27 +2063,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P1" sqref="P1"/>
+      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" style="14" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="18" width="32.42578125" style="1" customWidth="1"/>
@@ -4056,11 +4056,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
corrected the station details field
</commit_message>
<xml_diff>
--- a/Reading_TTC_Excel/excel_files/TestOneTrain.xlsx
+++ b/Reading_TTC_Excel/excel_files/TestOneTrain.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Yonge-University" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="435">
   <si>
     <t>Line 1 Yonge-University has 32 stations, and is a “U-shaped” route running generally in a south and then north direction. The route operates from the northern area of Yonge Street and Finch Avenue East, south to Union Station in downtown Toronto, and then north again to the area of Allen Road and Sheppard Avenue West. Line 1 connects with Line 2 at Bloor-Yonge, St George and Spadina stations, and it connects with Line 4 at Sheppard-Yonge Station.</t>
   </si>
@@ -198,9 +198,6 @@
 Accessible: Yes
 Number of Levels: 3
 Platform Type: Centre</t>
-  </si>
-  <si>
-    <t>Longitude</t>
   </si>
   <si>
     <t>6:21 am@6:28 am@8:30 am</t>
@@ -2066,11 +2063,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2087,8 +2084,8 @@
     <col min="10" max="10" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="18" width="32.42578125" style="1" customWidth="1"/>
     <col min="19" max="19" width="32.42578125" style="2" customWidth="1"/>
     <col min="20" max="21" width="32.42578125" style="12" customWidth="1"/>
@@ -2100,76 +2097,76 @@
   <sheetData>
     <row r="1" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>425</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>428</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="17" t="s">
         <v>429</v>
       </c>
-      <c r="T1" s="17" t="s">
-        <v>430</v>
-      </c>
       <c r="U1" s="17" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="V1" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>432</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>434</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="150" x14ac:dyDescent="0.25">
@@ -2180,7 +2177,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>38</v>
@@ -2210,10 +2207,10 @@
         <v>37</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="U2" s="11" t="s">
         <v>44</v>
@@ -2242,7 +2239,7 @@
         <v>40</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>41</v>
@@ -2272,7 +2269,7 @@
         <v>42</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T3" s="11" t="s">
         <v>43</v>
@@ -2328,7 +2325,7 @@
         <v>42</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T4" s="11" t="s">
         <v>50</v>
@@ -2387,7 +2384,7 @@
         <v>42</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T5" s="11" t="s">
         <v>55</v>
@@ -2410,17 +2407,17 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="K6" s="1" t="s">
         <v>42</v>
       </c>
@@ -2446,10 +2443,10 @@
         <v>42</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U6" s="12" t="s">
         <v>42</v>
@@ -2469,17 +2466,17 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="K7" s="1" t="s">
         <v>37</v>
       </c>
@@ -2505,10 +2502,10 @@
         <v>42</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U7" s="12" t="s">
         <v>42</v>
@@ -2528,17 +2525,17 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="K8" s="1" t="s">
         <v>42</v>
       </c>
@@ -2564,10 +2561,10 @@
         <v>42</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T8" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="U8" s="12" t="s">
         <v>42</v>
@@ -2587,16 +2584,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>42</v>
@@ -2623,10 +2620,10 @@
         <v>42</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T9" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="U9" s="12" t="s">
         <v>42</v>
@@ -2646,46 +2643,46 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="K10" t="s">
+        <v>74</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T10" s="11" t="s">
         <v>115</v>
-      </c>
-      <c r="K10" t="s">
-        <v>75</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="T10" s="11" t="s">
-        <v>116</v>
       </c>
       <c r="U10" s="12" t="s">
         <v>42</v>
@@ -2705,46 +2702,46 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="K11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="T11" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="T11" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="U11" s="12" t="s">
         <v>42</v>
@@ -2764,46 +2761,46 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="K12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="T12" s="11" t="s">
         <v>125</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="T12" s="11" t="s">
-        <v>126</v>
       </c>
       <c r="U12" s="12" t="s">
         <v>42</v>
@@ -2823,17 +2820,17 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="K13" s="1" t="s">
         <v>37</v>
       </c>
@@ -2859,10 +2856,10 @@
         <v>42</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T13" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U13" s="12" t="s">
         <v>42</v>
@@ -2882,17 +2879,17 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="K14" s="1" t="s">
         <v>42</v>
       </c>
@@ -2918,10 +2915,10 @@
         <v>37</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T14" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U14" s="12" t="s">
         <v>42</v>
@@ -2941,17 +2938,17 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="K15" s="1" t="s">
         <v>37</v>
       </c>
@@ -2977,10 +2974,10 @@
         <v>37</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T15" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U15" s="12" t="s">
         <v>42</v>
@@ -3000,17 +2997,17 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="K16" s="1" t="s">
         <v>37</v>
       </c>
@@ -3036,10 +3033,10 @@
         <v>42</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T16" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U16" s="12" t="s">
         <v>42</v>
@@ -3059,17 +3056,17 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="K17" s="1" t="s">
         <v>37</v>
       </c>
@@ -3095,10 +3092,10 @@
         <v>37</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T17" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U17" s="12" t="s">
         <v>42</v>
@@ -3118,16 +3115,16 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>42</v>
@@ -3154,10 +3151,10 @@
         <v>37</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T18" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U18" s="11" t="s">
         <v>42</v>
@@ -3177,16 +3174,16 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>37</v>
@@ -3213,10 +3210,10 @@
         <v>37</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T19" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="U19" s="12" t="s">
         <v>42</v>
@@ -3236,17 +3233,17 @@
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="K20" s="1" t="s">
         <v>37</v>
       </c>
@@ -3272,10 +3269,10 @@
         <v>37</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T20" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U20" s="12" t="s">
         <v>42</v>
@@ -3295,16 +3292,16 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>42</v>
@@ -3331,10 +3328,10 @@
         <v>37</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T21" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U21" s="12" t="s">
         <v>42</v>
@@ -3354,16 +3351,16 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>42</v>
@@ -3390,10 +3387,10 @@
         <v>42</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T22" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="U22" s="12" t="s">
         <v>42</v>
@@ -3413,16 +3410,16 @@
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>37</v>
@@ -3449,10 +3446,10 @@
         <v>37</v>
       </c>
       <c r="S23" t="s">
+        <v>91</v>
+      </c>
+      <c r="T23" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="U23" s="12" t="s">
         <v>42</v>
@@ -3472,16 +3469,16 @@
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>42</v>
@@ -3508,10 +3505,10 @@
         <v>42</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T24" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U24" s="12" t="s">
         <v>42</v>
@@ -3531,17 +3528,17 @@
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="K25" s="1" t="s">
         <v>42</v>
       </c>
@@ -3567,10 +3564,10 @@
         <v>42</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T25" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U25" s="12" t="s">
         <v>42</v>
@@ -3590,16 +3587,16 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>37</v>
@@ -3626,10 +3623,10 @@
         <v>37</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T26" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U26" s="12" t="s">
         <v>42</v>
@@ -3649,17 +3646,17 @@
         <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="K27" s="1" t="s">
         <v>37</v>
       </c>
@@ -3685,10 +3682,10 @@
         <v>37</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T27" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U27" s="12" t="s">
         <v>42</v>
@@ -3708,46 +3705,46 @@
         <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S28" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="T28" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="U28" s="12" t="s">
         <v>42</v>
@@ -3767,17 +3764,17 @@
         <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="K29" s="1" t="s">
         <v>42</v>
       </c>
@@ -3800,10 +3797,10 @@
         <v>42</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T29" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="U29" s="12" t="s">
         <v>42</v>
@@ -3823,17 +3820,17 @@
         <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="K30" s="1" t="s">
         <v>37</v>
       </c>
@@ -3859,10 +3856,10 @@
         <v>37</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T30" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U30" s="12" t="s">
         <v>42</v>
@@ -3882,17 +3879,17 @@
         <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="K31" s="1" t="s">
         <v>37</v>
       </c>
@@ -3918,10 +3915,10 @@
         <v>37</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T31" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U31" s="12" t="s">
         <v>42</v>
@@ -3941,13 +3938,13 @@
         <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>38</v>
@@ -3977,10 +3974,10 @@
         <v>37</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T32" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U32" s="12" t="s">
         <v>42</v>
@@ -4000,10 +3997,10 @@
         <v>32</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -4034,13 +4031,13 @@
         <v>37</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T33" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="U33" s="11" t="s">
         <v>103</v>
-      </c>
-      <c r="U33" s="11" t="s">
-        <v>104</v>
       </c>
       <c r="V33" s="2">
         <v>43.780467000000002</v>
@@ -4059,11 +4056,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4095,90 +4092,90 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>425</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>428</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="17" t="s">
         <v>429</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>430</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="13" t="s">
         <v>431</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>432</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>434</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>37</v>
@@ -4205,13 +4202,13 @@
         <v>37</v>
       </c>
       <c r="S2" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="U2" s="11" t="s">
         <v>212</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>213</v>
       </c>
       <c r="V2" s="2">
         <v>43.638491000000002</v>
@@ -4225,23 +4222,23 @@
     </row>
     <row r="3" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="K3" s="2" t="s">
         <v>42</v>
       </c>
@@ -4267,13 +4264,13 @@
         <v>37</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="T3" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="U3" s="11" t="s">
         <v>215</v>
-      </c>
-      <c r="U3" s="11" t="s">
-        <v>216</v>
       </c>
       <c r="V3" s="2">
         <v>43.645274999999998</v>
@@ -4284,23 +4281,23 @@
     </row>
     <row r="4" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>284</v>
-      </c>
       <c r="K4" s="2" t="s">
         <v>42</v>
       </c>
@@ -4326,10 +4323,10 @@
         <v>42</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="U4" s="11" t="s">
         <v>42</v>
@@ -4343,23 +4340,23 @@
     </row>
     <row r="5" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="K5" s="2" t="s">
         <v>42</v>
       </c>
@@ -4385,10 +4382,10 @@
         <v>42</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U5" s="11" t="s">
         <v>42</v>
@@ -4402,23 +4399,23 @@
     </row>
     <row r="6" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>289</v>
-      </c>
       <c r="K6" s="2" t="s">
         <v>37</v>
       </c>
@@ -4444,10 +4441,10 @@
         <v>42</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U6" s="11" t="s">
         <v>42</v>
@@ -4461,23 +4458,23 @@
     </row>
     <row r="7" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>293</v>
-      </c>
       <c r="K7" s="2" t="s">
         <v>42</v>
       </c>
@@ -4503,10 +4500,10 @@
         <v>42</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U7" s="11" t="s">
         <v>42</v>
@@ -4520,22 +4517,22 @@
     </row>
     <row r="8" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>295</v>
-      </c>
       <c r="J8" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>42</v>
@@ -4562,10 +4559,10 @@
         <v>42</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U8" s="11" t="s">
         <v>42</v>
@@ -4579,22 +4576,22 @@
     </row>
     <row r="9" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>297</v>
-      </c>
       <c r="J9" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>42</v>
@@ -4621,13 +4618,13 @@
         <v>42</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T9" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="U9" s="11" t="s">
         <v>222</v>
-      </c>
-      <c r="U9" s="11" t="s">
-        <v>223</v>
       </c>
       <c r="V9" s="2">
         <v>43.655462</v>
@@ -4638,23 +4635,23 @@
     </row>
     <row r="10" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>301</v>
-      </c>
       <c r="K10" s="2" t="s">
         <v>37</v>
       </c>
@@ -4680,10 +4677,10 @@
         <v>37</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U10" s="11" t="s">
         <v>42</v>
@@ -4697,19 +4694,19 @@
     </row>
     <row r="11" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>303</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>52</v>
@@ -4739,10 +4736,10 @@
         <v>42</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U11" s="11" t="s">
         <v>42</v>
@@ -4756,22 +4753,22 @@
     </row>
     <row r="12" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>305</v>
-      </c>
       <c r="J12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>37</v>
@@ -4798,10 +4795,10 @@
         <v>42</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="U12" s="11" t="s">
         <v>42</v>
@@ -4815,23 +4812,23 @@
     </row>
     <row r="13" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>309</v>
-      </c>
       <c r="K13" s="2" t="s">
         <v>42</v>
       </c>
@@ -4857,10 +4854,10 @@
         <v>37</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="U13" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="V13" s="2">
         <v>43.662436999999997</v>
@@ -4871,23 +4868,23 @@
     </row>
     <row r="14" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="K14" s="2" t="s">
         <v>42</v>
       </c>
@@ -4913,10 +4910,10 @@
         <v>42</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="U14" s="11" t="s">
         <v>42</v>
@@ -4930,23 +4927,23 @@
     </row>
     <row r="15" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>317</v>
-      </c>
       <c r="K15" s="2" t="s">
         <v>37</v>
       </c>
@@ -4972,10 +4969,10 @@
         <v>37</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="U15" s="11" t="s">
         <v>42</v>
@@ -4995,46 +4992,46 @@
         <v>15</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>321</v>
-      </c>
       <c r="K16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S16" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="T16" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="U16" s="11" t="s">
         <v>42</v>
@@ -5048,23 +5045,23 @@
     </row>
     <row r="17" spans="1:23" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>325</v>
-      </c>
       <c r="K17" s="2" t="s">
         <v>37</v>
       </c>
@@ -5090,10 +5087,10 @@
         <v>37</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="U17" s="11" t="s">
         <v>42</v>
@@ -5107,22 +5104,22 @@
     </row>
     <row r="18" spans="1:23" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>328</v>
-      </c>
       <c r="J18" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>42</v>
@@ -5149,10 +5146,10 @@
         <v>37</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="U18" s="11" t="s">
         <v>42</v>
@@ -5166,22 +5163,22 @@
     </row>
     <row r="19" spans="1:23" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B19" s="2">
         <v>18</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>330</v>
-      </c>
       <c r="J19" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>37</v>
@@ -5208,10 +5205,10 @@
         <v>37</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T19" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U19" s="11" t="s">
         <v>42</v>
@@ -5225,22 +5222,22 @@
     </row>
     <row r="20" spans="1:23" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B20" s="2">
         <v>19</v>
       </c>
       <c r="G20" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>332</v>
-      </c>
       <c r="J20" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>42</v>
@@ -5267,10 +5264,10 @@
         <v>37</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U20" s="11" t="s">
         <v>42</v>
@@ -5284,23 +5281,23 @@
     </row>
     <row r="21" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B21" s="2">
         <v>20</v>
       </c>
       <c r="G21" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>336</v>
-      </c>
       <c r="K21" s="2" t="s">
         <v>42</v>
       </c>
@@ -5326,10 +5323,10 @@
         <v>42</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U21" s="11" t="s">
         <v>42</v>
@@ -5343,23 +5340,23 @@
     </row>
     <row r="22" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B22" s="2">
         <v>21</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="I22" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>339</v>
-      </c>
       <c r="K22" s="2" t="s">
         <v>37</v>
       </c>
@@ -5385,10 +5382,10 @@
         <v>37</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T22" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="U22" s="11" t="s">
         <v>42</v>
@@ -5402,23 +5399,23 @@
     </row>
     <row r="23" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B23" s="2">
         <v>22</v>
       </c>
       <c r="G23" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>343</v>
-      </c>
       <c r="K23" s="2" t="s">
         <v>42</v>
       </c>
@@ -5444,10 +5441,10 @@
         <v>42</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T23" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U23" s="11" t="s">
         <v>42</v>
@@ -5461,23 +5458,23 @@
     </row>
     <row r="24" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B24" s="2">
         <v>23</v>
       </c>
       <c r="G24" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>347</v>
-      </c>
       <c r="K24" s="2" t="s">
         <v>37</v>
       </c>
@@ -5503,10 +5500,10 @@
         <v>42</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U24" s="11" t="s">
         <v>42</v>
@@ -5520,23 +5517,23 @@
     </row>
     <row r="25" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B25" s="2">
         <v>24</v>
       </c>
       <c r="G25" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="J25" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="J25" s="2" t="s">
-        <v>351</v>
-      </c>
       <c r="K25" s="2" t="s">
         <v>42</v>
       </c>
@@ -5562,10 +5559,10 @@
         <v>42</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U25" s="11" t="s">
         <v>42</v>
@@ -5579,23 +5576,23 @@
     </row>
     <row r="26" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B26" s="2">
         <v>25</v>
       </c>
       <c r="G26" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="J26" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="J26" s="2" t="s">
-        <v>355</v>
-      </c>
       <c r="K26" s="2" t="s">
         <v>42</v>
       </c>
@@ -5621,10 +5618,10 @@
         <v>42</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T26" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="U26" s="11" t="s">
         <v>42</v>
@@ -5638,23 +5635,23 @@
     </row>
     <row r="27" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B27" s="2">
         <v>26</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="J27" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>359</v>
-      </c>
       <c r="K27" s="2" t="s">
         <v>42</v>
       </c>
@@ -5680,10 +5677,10 @@
         <v>42</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="U27" s="11" t="s">
         <v>42</v>
@@ -5697,23 +5694,23 @@
     </row>
     <row r="28" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B28" s="2">
         <v>27</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="J28" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>363</v>
-      </c>
       <c r="K28" s="2" t="s">
         <v>42</v>
       </c>
@@ -5739,10 +5736,10 @@
         <v>42</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T28" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="U28" s="11" t="s">
         <v>42</v>
@@ -5756,23 +5753,23 @@
     </row>
     <row r="29" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B29" s="2">
         <v>28</v>
       </c>
       <c r="G29" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="J29" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>367</v>
-      </c>
       <c r="K29" s="2" t="s">
         <v>37</v>
       </c>
@@ -5798,10 +5795,10 @@
         <v>37</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T29" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="U29" s="11" t="s">
         <v>42</v>
@@ -5815,23 +5812,23 @@
     </row>
     <row r="30" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B30" s="2">
         <v>29</v>
       </c>
       <c r="G30" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="J30" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>371</v>
-      </c>
       <c r="K30" s="2" t="s">
         <v>37</v>
       </c>
@@ -5857,13 +5854,13 @@
         <v>42</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T30" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="U30" s="11" t="s">
         <v>249</v>
-      </c>
-      <c r="U30" s="11" t="s">
-        <v>250</v>
       </c>
       <c r="V30" s="2">
         <v>43.694043999999998</v>
@@ -5874,23 +5871,23 @@
     </row>
     <row r="31" spans="1:23" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B31" s="2">
         <v>30</v>
       </c>
       <c r="G31" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="J31" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="J31" s="2" t="s">
-        <v>375</v>
-      </c>
       <c r="K31" s="2" t="s">
         <v>42</v>
       </c>
@@ -5916,13 +5913,13 @@
         <v>37</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="T31" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="U31" s="11" t="s">
         <v>251</v>
-      </c>
-      <c r="U31" s="11" t="s">
-        <v>252</v>
       </c>
       <c r="V31" s="2">
         <v>43.710965000000002</v>
@@ -5933,23 +5930,23 @@
     </row>
     <row r="32" spans="1:23" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B32" s="2">
         <v>31</v>
       </c>
       <c r="G32" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="J32" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="J32" s="2" t="s">
-        <v>379</v>
-      </c>
       <c r="K32" s="2" t="s">
         <v>37</v>
       </c>
@@ -5975,13 +5972,13 @@
         <v>37</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="T32" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="U32" s="11" t="s">
         <v>253</v>
-      </c>
-      <c r="U32" s="11" t="s">
-        <v>254</v>
       </c>
       <c r="V32" s="2">
         <v>43.732269000000002</v>
@@ -6004,7 +6001,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6030,104 +6027,104 @@
     <col min="20" max="20" width="35.140625" style="11" customWidth="1"/>
     <col min="21" max="21" width="29.42578125" style="12" customWidth="1"/>
     <col min="22" max="22" width="16.28515625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="64" style="2" customWidth="1"/>
     <col min="25" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>425</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>428</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="17" t="s">
         <v>429</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>430</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="13" t="s">
         <v>431</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>432</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>379</v>
-      </c>
       <c r="K2" s="2" t="s">
         <v>37</v>
       </c>
@@ -6153,13 +6150,13 @@
         <v>37</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T2" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="U2" s="11" t="s">
         <v>253</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>254</v>
       </c>
       <c r="V2" s="2">
         <v>43.732269000000002</v>
@@ -6173,23 +6170,23 @@
     </row>
     <row r="3" spans="1:24" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>382</v>
-      </c>
       <c r="K3" s="2" t="s">
         <v>42</v>
       </c>
@@ -6215,13 +6212,13 @@
         <v>42</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T3" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="U3" s="11" t="s">
         <v>260</v>
-      </c>
-      <c r="U3" s="11" t="s">
-        <v>261</v>
       </c>
       <c r="V3" s="2">
         <v>43.750492999999999</v>
@@ -6232,23 +6229,23 @@
     </row>
     <row r="4" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>386</v>
-      </c>
       <c r="K4" s="2" t="s">
         <v>42</v>
       </c>
@@ -6274,13 +6271,13 @@
         <v>42</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T4" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="U4" s="11" t="s">
         <v>262</v>
-      </c>
-      <c r="U4" s="11" t="s">
-        <v>263</v>
       </c>
       <c r="V4" s="2">
         <v>43.76688</v>
@@ -6291,23 +6288,23 @@
     </row>
     <row r="5" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>390</v>
-      </c>
       <c r="K5" s="2" t="s">
         <v>42</v>
       </c>
@@ -6333,10 +6330,10 @@
         <v>42</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="U5" s="12" t="s">
         <v>42</v>
@@ -6350,23 +6347,23 @@
     </row>
     <row r="6" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>393</v>
-      </c>
       <c r="K6" s="2" t="s">
         <v>37</v>
       </c>
@@ -6392,10 +6389,10 @@
         <v>37</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="U6" s="12" t="s">
         <v>42</v>
@@ -6409,17 +6406,17 @@
     </row>
     <row r="7" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>395</v>
-      </c>
       <c r="K7" s="2" t="s">
         <v>42</v>
       </c>
@@ -6445,10 +6442,10 @@
         <v>42</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="U7" s="12" t="s">
         <v>42</v>
@@ -6504,91 +6501,91 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>425</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>428</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="17" t="s">
         <v>429</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>430</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="13" t="s">
         <v>431</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>432</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>397</v>
-      </c>
       <c r="K2" s="2" t="s">
         <v>37</v>
       </c>
@@ -6614,10 +6611,10 @@
         <v>37</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U2" s="12" t="s">
         <v>42</v>
@@ -6634,23 +6631,23 @@
     </row>
     <row r="3" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>401</v>
-      </c>
       <c r="K3" s="2" t="s">
         <v>37</v>
       </c>
@@ -6676,10 +6673,10 @@
         <v>42</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="T3" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="U3" s="12" t="s">
         <v>42</v>
@@ -6693,23 +6690,23 @@
     </row>
     <row r="4" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>405</v>
-      </c>
       <c r="K4" s="2" t="s">
         <v>37</v>
       </c>
@@ -6735,10 +6732,10 @@
         <v>42</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="U4" s="12" t="s">
         <v>42</v>
@@ -6752,23 +6749,23 @@
     </row>
     <row r="5" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>409</v>
-      </c>
       <c r="K5" s="2" t="s">
         <v>37</v>
       </c>
@@ -6794,13 +6791,13 @@
         <v>42</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="T5" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="U5" s="12" t="s">
         <v>274</v>
-      </c>
-      <c r="U5" s="12" t="s">
-        <v>275</v>
       </c>
       <c r="V5" s="2">
         <v>43.770409999999998</v>
@@ -6811,17 +6808,17 @@
     </row>
     <row r="6" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>411</v>
-      </c>
       <c r="K6" s="2" t="s">
         <v>37</v>
       </c>
@@ -6847,13 +6844,13 @@
         <v>37</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="T6" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="U6" s="12" t="s">
         <v>276</v>
-      </c>
-      <c r="U6" s="12" t="s">
-        <v>277</v>
       </c>
       <c r="V6" s="2">
         <v>43.775593000000001</v>

</xml_diff>

<commit_message>
Decorative patten test four
</commit_message>
<xml_diff>
--- a/Reading_TTC_Excel/excel_files/TestOneTrain.xlsx
+++ b/Reading_TTC_Excel/excel_files/TestOneTrain.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="434">
   <si>
     <t>Line 1 Yonge-University has 32 stations, and is a “U-shaped” route running generally in a south and then north direction. The route operates from the northern area of Yonge Street and Finch Avenue East, south to Union Station in downtown Toronto, and then north again to the area of Allen Road and Sheppard Avenue West. Line 1 connects with Line 2 at Bloor-Yonge, St George and Spadina stations, and it connects with Line 4 at Sheppard-Yonge Station.</t>
   </si>
@@ -1130,9 +1130,6 @@
     <t>5:43 am@5:50 am@8:03 am</t>
   </si>
   <si>
-    <t>6:02 am@:02 am@8:32 am</t>
-  </si>
-  <si>
     <t>2:14 am@2:14 am@2:14 am</t>
   </si>
   <si>
@@ -1593,6 +1590,9 @@
   </si>
   <si>
     <t>LONGITUDE</t>
+  </si>
+  <si>
+    <t>6:02 am@6:02 am@8:32 am</t>
   </si>
 </sst>
 </file>
@@ -2061,24 +2061,23 @@
   <dimension ref="A1:X33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" style="14" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -2094,76 +2093,76 @@
   <sheetData>
     <row r="1" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="13" t="s">
         <v>421</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>425</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="17" t="s">
         <v>428</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>429</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="13" t="s">
         <v>430</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>431</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>433</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="150" x14ac:dyDescent="0.25">
@@ -2651,6 +2650,18 @@
       <c r="F10" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="G10" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>319</v>
+      </c>
       <c r="K10" t="s">
         <v>74</v>
       </c>
@@ -3886,6 +3897,12 @@
       </c>
       <c r="F31" s="1" t="s">
         <v>184</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>395</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>37</v>
@@ -4054,10 +4071,10 @@
   <dimension ref="A1:X32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V1" sqref="V1"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4089,76 +4106,76 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="13" t="s">
         <v>421</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>425</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="17" t="s">
         <v>428</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>429</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="13" t="s">
         <v>430</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>431</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>433</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4231,10 +4248,10 @@
         <v>164</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>42</v>
@@ -4284,16 +4301,16 @@
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>70</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>42</v>
@@ -4343,16 +4360,16 @@
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>124</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>42</v>
@@ -4402,16 +4419,16 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>37</v>
@@ -4461,16 +4478,16 @@
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>292</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>42</v>
@@ -4520,13 +4537,13 @@
         <v>7</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>133</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>178</v>
@@ -4579,13 +4596,13 @@
         <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>137</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>174</v>
@@ -4632,22 +4649,22 @@
     </row>
     <row r="10" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>135</v>
       </c>
       <c r="I10" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>37</v>
@@ -4697,13 +4714,13 @@
         <v>10</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>131</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>52</v>
@@ -4756,13 +4773,13 @@
         <v>11</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>143</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>57</v>
@@ -4815,16 +4832,16 @@
         <v>12</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>307</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>308</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>42</v>
@@ -4871,16 +4888,16 @@
         <v>13</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>312</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>42</v>
@@ -4930,16 +4947,16 @@
         <v>14</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>316</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>37</v>
@@ -4989,16 +5006,16 @@
         <v>15</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>319</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>320</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>74</v>
@@ -5048,16 +5065,16 @@
         <v>16</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>324</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>37</v>
@@ -5107,16 +5124,16 @@
         <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>327</v>
-      </c>
       <c r="J18" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>42</v>
@@ -5166,16 +5183,16 @@
         <v>18</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>329</v>
-      </c>
       <c r="J19" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>37</v>
@@ -5225,16 +5242,16 @@
         <v>19</v>
       </c>
       <c r="G20" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>331</v>
-      </c>
       <c r="J20" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>42</v>
@@ -5284,16 +5301,16 @@
         <v>20</v>
       </c>
       <c r="G21" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>42</v>
@@ -5343,16 +5360,16 @@
         <v>21</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="I22" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>338</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>37</v>
@@ -5402,16 +5419,16 @@
         <v>22</v>
       </c>
       <c r="G23" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>341</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>342</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>42</v>
@@ -5461,16 +5478,16 @@
         <v>23</v>
       </c>
       <c r="G24" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>346</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>37</v>
@@ -5520,16 +5537,16 @@
         <v>24</v>
       </c>
       <c r="G25" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="J25" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>350</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>42</v>
@@ -5579,16 +5596,16 @@
         <v>25</v>
       </c>
       <c r="G26" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="J26" s="2" t="s">
         <v>353</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>354</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>42</v>
@@ -5638,16 +5655,16 @@
         <v>26</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="J27" s="2" t="s">
         <v>357</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>358</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>42</v>
@@ -5697,16 +5714,16 @@
         <v>27</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="J28" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>362</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>42</v>
@@ -5756,16 +5773,16 @@
         <v>28</v>
       </c>
       <c r="G29" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="J29" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>366</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>37</v>
@@ -5815,16 +5832,16 @@
         <v>29</v>
       </c>
       <c r="G30" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="J30" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>370</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>37</v>
@@ -5874,16 +5891,16 @@
         <v>30</v>
       </c>
       <c r="G31" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="J31" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>374</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>42</v>
@@ -5933,16 +5950,16 @@
         <v>31</v>
       </c>
       <c r="G32" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="J32" s="2" t="s">
         <v>377</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>378</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>37</v>
@@ -5995,10 +6012,10 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6031,76 +6048,76 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="13" t="s">
         <v>421</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>425</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="17" t="s">
         <v>428</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>429</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="13" t="s">
         <v>430</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>431</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>433</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="195" x14ac:dyDescent="0.25">
@@ -6111,16 +6128,16 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>377</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>378</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>37</v>
@@ -6173,16 +6190,16 @@
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>381</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>42</v>
@@ -6232,16 +6249,16 @@
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>385</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>42</v>
@@ -6291,16 +6308,16 @@
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>389</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>42</v>
@@ -6350,16 +6367,16 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>392</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>37</v>
@@ -6409,10 +6426,10 @@
         <v>6</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>393</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>394</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>42</v>
@@ -6464,10 +6481,10 @@
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W7" sqref="W7"/>
+      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6498,76 +6515,76 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="13" t="s">
         <v>421</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>425</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="17" t="s">
         <v>428</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>429</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="13" t="s">
         <v>430</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>431</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>433</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="135" x14ac:dyDescent="0.25">
@@ -6577,11 +6594,23 @@
       <c r="B2" s="2">
         <v>1</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="G2" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>395</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>396</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>37</v>
@@ -6634,16 +6663,16 @@
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>400</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>37</v>
@@ -6693,16 +6722,16 @@
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>404</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>37</v>
@@ -6752,16 +6781,16 @@
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>37</v>
@@ -6811,10 +6840,10 @@
         <v>5</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>410</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
check duplicatest in the Arraylist
</commit_message>
<xml_diff>
--- a/Reading_TTC_Excel/excel_files/TestOneTrain.xlsx
+++ b/Reading_TTC_Excel/excel_files/TestOneTrain.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Yonge-University" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,15 @@
     <sheet name="Scarborough" sheetId="3" r:id="rId3"/>
     <sheet name="Sheppard " sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Bloor-Danforth'!$A$1:$X$32</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="430">
   <si>
     <t>Line 1 Yonge-University has 32 stations, and is a “U-shaped” route running generally in a south and then north direction. The route operates from the northern area of Yonge Street and Finch Avenue East, south to Union Station in downtown Toronto, and then north again to the area of Allen Road and Sheppard Avenue West. Line 1 connects with Line 2 at Bloor-Yonge, St George and Spadina stations, and it connects with Line 4 at Sheppard-Yonge Station.</t>
   </si>
@@ -872,12 +875,6 @@
     <t>Bathurst</t>
   </si>
   <si>
-    <t>St George</t>
-  </si>
-  <si>
-    <t>Bloor-Yonge</t>
-  </si>
-  <si>
     <t>Broadview</t>
   </si>
   <si>
@@ -1079,9 +1076,6 @@
     <t xml:space="preserve">Don Mills </t>
   </si>
   <si>
-    <t>Sheppard-Yonge</t>
-  </si>
-  <si>
     <t>Bayview</t>
   </si>
   <si>
@@ -1206,9 +1200,6 @@
   </si>
   <si>
     <t>5:57 am @ 6:04 am  @ 8:18 am</t>
-  </si>
-  <si>
-    <t>1:47 am  @ 1:47 am  Sunday 1:47 am</t>
   </si>
   <si>
     <t>5:56 am  @ 6:01 am  @ 8:17 am</t>
@@ -2060,11 +2051,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2093,76 +2084,76 @@
   <sheetData>
     <row r="1" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="H1" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="I1" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="J1" s="13" t="s">
         <v>414</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>416</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="P1" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>421</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="T1" s="17" t="s">
         <v>424</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="U1" s="17" t="s">
         <v>425</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="W1" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>427</v>
-      </c>
-      <c r="T1" s="17" t="s">
-        <v>428</v>
-      </c>
-      <c r="U1" s="17" t="s">
-        <v>429</v>
-      </c>
-      <c r="V1" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="150" x14ac:dyDescent="0.25">
@@ -2212,10 +2203,10 @@
         <v>44</v>
       </c>
       <c r="V2" s="5">
-        <v>43.749124000000002</v>
+        <v>43.749700168199702</v>
       </c>
       <c r="W2" s="5">
-        <v>-79.462194999999994</v>
+        <v>-79.461905546486307</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>0</v>
@@ -2274,10 +2265,10 @@
         <v>45</v>
       </c>
       <c r="V3" s="5">
-        <v>43.734515000000002</v>
+        <v>43.734465041446803</v>
       </c>
       <c r="W3" s="5">
-        <v>-79.450851</v>
+        <v>-79.450104162096906</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="165" x14ac:dyDescent="0.25">
@@ -2330,10 +2321,10 @@
         <v>42</v>
       </c>
       <c r="V4" s="2">
-        <v>43.724547999999999</v>
+        <v>43.724608843296203</v>
       </c>
       <c r="W4" s="2">
-        <v>-79.447485</v>
+        <v>-79.447514154016901</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="75" x14ac:dyDescent="0.25">
@@ -2389,10 +2380,10 @@
         <v>42</v>
       </c>
       <c r="V5" s="2">
-        <v>43.715620999999999</v>
+        <v>43.715592158579902</v>
       </c>
       <c r="W5" s="2">
-        <v>-79.444027000000006</v>
+        <v>-79.444042034447193</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -2448,10 +2439,10 @@
         <v>42</v>
       </c>
       <c r="V6" s="2">
-        <v>43.709611000000002</v>
+        <v>43.708778647031103</v>
       </c>
       <c r="W6" s="2">
-        <v>-79.441321000000002</v>
+        <v>-79.440727829933095</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="75" x14ac:dyDescent="0.25">
@@ -2507,10 +2498,10 @@
         <v>42</v>
       </c>
       <c r="V7" s="2">
-        <v>43.699370000000002</v>
+        <v>43.699369808375799</v>
       </c>
       <c r="W7" s="2">
-        <v>-79.436091000000005</v>
+        <v>-79.436147622764096</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -2566,10 +2557,10 @@
         <v>42</v>
       </c>
       <c r="V8" s="2">
-        <v>43.684375000000003</v>
+        <v>43.684085266843098</v>
       </c>
       <c r="W8" s="2">
-        <v>-79.415034000000006</v>
+        <v>-79.415719583630505</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -2625,10 +2616,10 @@
         <v>42</v>
       </c>
       <c r="V9" s="2">
-        <v>43.674734000000001</v>
+        <v>43.674854909847802</v>
       </c>
       <c r="W9" s="2">
-        <v>-79.406824999999998</v>
+        <v>-79.407079853117395</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="195" x14ac:dyDescent="0.25">
@@ -2651,16 +2642,16 @@
         <v>114</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="K10" t="s">
         <v>74</v>
@@ -2721,6 +2712,18 @@
       <c r="F11" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="G11" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>319</v>
+      </c>
       <c r="K11" s="1" t="s">
         <v>37</v>
       </c>
@@ -2755,10 +2758,10 @@
         <v>42</v>
       </c>
       <c r="V11" s="2">
-        <v>43.668678999999997</v>
+        <v>43.668263526774602</v>
       </c>
       <c r="W11" s="2">
-        <v>-79.397909999999996</v>
+        <v>-79.399852640926795</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -2814,10 +2817,10 @@
         <v>42</v>
       </c>
       <c r="V12" s="2">
-        <v>43.666977000000003</v>
+        <v>43.667120995267098</v>
       </c>
       <c r="W12" s="2">
-        <v>-79.393540999999999</v>
+        <v>-79.393466301262293</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -2873,10 +2876,10 @@
         <v>42</v>
       </c>
       <c r="V13" s="2">
-        <v>43.659669999999998</v>
+        <v>43.659882112658202</v>
       </c>
       <c r="W13" s="2">
-        <v>-79.390777999999997</v>
+        <v>-79.390469267964306</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -2932,10 +2935,10 @@
         <v>42</v>
       </c>
       <c r="V14" s="2">
-        <v>43.654972999999998</v>
+        <v>43.654825582494297</v>
       </c>
       <c r="W14" s="2">
-        <v>-79.388098999999997</v>
+        <v>-79.388339594006496</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -2991,10 +2994,10 @@
         <v>42</v>
       </c>
       <c r="V15" s="2">
-        <v>43.651010999999997</v>
+        <v>43.650840408766797</v>
       </c>
       <c r="W15" s="2">
-        <v>-79.386958000000007</v>
+        <v>-79.386590458452702</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -3050,10 +3053,10 @@
         <v>42</v>
       </c>
       <c r="V16" s="2">
-        <v>43.647458999999998</v>
+        <v>43.647523110342497</v>
       </c>
       <c r="W16" s="2">
-        <v>-79.385157000000007</v>
+        <v>-79.3844842538237</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="90" x14ac:dyDescent="0.25">
@@ -3109,10 +3112,10 @@
         <v>42</v>
       </c>
       <c r="V17" s="2">
-        <v>43.645211000000003</v>
+        <v>43.6452238923358</v>
       </c>
       <c r="W17" s="2">
-        <v>-79.380784000000006</v>
+        <v>-79.380854889750395</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -3168,10 +3171,10 @@
         <v>42</v>
       </c>
       <c r="V18" s="2">
-        <v>43.649273000000001</v>
+        <v>43.648992554955598</v>
       </c>
       <c r="W18" s="2">
-        <v>-79.377996999999993</v>
+        <v>-79.377792812883797</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -3227,10 +3230,10 @@
         <v>42</v>
       </c>
       <c r="V19" s="2">
-        <v>43.652509999999999</v>
+        <v>43.652424758040098</v>
       </c>
       <c r="W19" s="2">
-        <v>-79.379340999999997</v>
+        <v>-79.379244893789206</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="135" x14ac:dyDescent="0.25">
@@ -3286,10 +3289,10 @@
         <v>42</v>
       </c>
       <c r="V20" s="2">
-        <v>43.65643</v>
+        <v>43.656247304661598</v>
       </c>
       <c r="W20" s="2">
-        <v>-79.380818000000005</v>
+        <v>-79.380886405706406</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -3345,10 +3348,10 @@
         <v>42</v>
       </c>
       <c r="V21" s="2">
-        <v>43.661259999999999</v>
+        <v>43.661326757351098</v>
       </c>
       <c r="W21" s="2">
-        <v>-79.383224999999996</v>
+        <v>-79.383062683045793</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="135" x14ac:dyDescent="0.25">
@@ -3404,10 +3407,10 @@
         <v>42</v>
       </c>
       <c r="V22" s="2">
-        <v>43.665244999999999</v>
+        <v>43.6654550575633</v>
       </c>
       <c r="W22" s="2">
-        <v>-79.383679000000001</v>
+        <v>-79.383888468146296</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="180" x14ac:dyDescent="0.25">
@@ -3429,6 +3432,18 @@
       <c r="F23" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="G23" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>317</v>
+      </c>
       <c r="K23" s="1" t="s">
         <v>37</v>
       </c>
@@ -3463,10 +3478,10 @@
         <v>42</v>
       </c>
       <c r="V23" s="2">
-        <v>43.670561999999997</v>
+        <v>43.670934603459003</v>
       </c>
       <c r="W23" s="2">
-        <v>-79.386402000000004</v>
+        <v>-79.385901130735803</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="120" x14ac:dyDescent="0.25">
@@ -3522,10 +3537,10 @@
         <v>42</v>
       </c>
       <c r="V24" s="2">
-        <v>43.676839999999999</v>
+        <v>43.6768935328544</v>
       </c>
       <c r="W24" s="2">
-        <v>-79.388874999999999</v>
+        <v>-79.388699680566702</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -3640,10 +3655,10 @@
         <v>42</v>
       </c>
       <c r="V26" s="2">
-        <v>43.687795999999999</v>
+        <v>43.687610259488601</v>
       </c>
       <c r="W26" s="2">
-        <v>-79.392202999999995</v>
+        <v>-79.393062293529496</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="120" x14ac:dyDescent="0.25">
@@ -3699,10 +3714,10 @@
         <v>42</v>
       </c>
       <c r="V27" s="2">
-        <v>43.697941999999998</v>
+        <v>43.697687797744301</v>
       </c>
       <c r="W27" s="2">
-        <v>-79.396671999999995</v>
+        <v>-79.397180825471807</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="120" x14ac:dyDescent="0.25">
@@ -3758,10 +3773,10 @@
         <v>42</v>
       </c>
       <c r="V28" s="2">
-        <v>43.705432999999999</v>
+        <v>43.706158940743897</v>
       </c>
       <c r="W28" s="2">
-        <v>-79.398742999999996</v>
+        <v>-79.398324452340603</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -3814,10 +3829,10 @@
         <v>42</v>
       </c>
       <c r="V29" s="2">
-        <v>43.725518000000001</v>
+        <v>43.726575512328601</v>
       </c>
       <c r="W29" s="2">
-        <v>-79.402367999999996</v>
+        <v>-79.402610287070203</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="150" x14ac:dyDescent="0.25">
@@ -3873,10 +3888,10 @@
         <v>42</v>
       </c>
       <c r="V30" s="2">
-        <v>43.744849000000002</v>
+        <v>43.744620689374997</v>
       </c>
       <c r="W30" s="2">
-        <v>-79.406415999999993</v>
+        <v>-79.406305029988204</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="195" x14ac:dyDescent="0.25">
@@ -3899,10 +3914,10 @@
         <v>184</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>37</v>
@@ -3938,10 +3953,10 @@
         <v>42</v>
       </c>
       <c r="V31" s="2">
-        <v>43.761564</v>
+        <v>43.762033524372697</v>
       </c>
       <c r="W31" s="2">
-        <v>-79.412107000000006</v>
+        <v>-79.411892406642394</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -4054,10 +4069,10 @@
         <v>103</v>
       </c>
       <c r="V33" s="2">
-        <v>43.780467000000002</v>
+        <v>43.781648950700998</v>
       </c>
       <c r="W33" s="2">
-        <v>-79.414636000000002</v>
+        <v>-79.415656886994796</v>
       </c>
     </row>
   </sheetData>
@@ -4071,10 +4086,10 @@
   <dimension ref="A1:X32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16:J16"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4087,7 +4102,7 @@
     <col min="6" max="6" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="38.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="32.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -4106,76 +4121,76 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="H1" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="I1" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="J1" s="13" t="s">
         <v>414</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>416</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="P1" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>421</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="T1" s="17" t="s">
         <v>424</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="U1" s="17" t="s">
         <v>425</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="W1" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>427</v>
-      </c>
-      <c r="T1" s="17" t="s">
-        <v>428</v>
-      </c>
-      <c r="U1" s="17" t="s">
-        <v>429</v>
-      </c>
-      <c r="V1" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4186,7 +4201,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>69</v>
@@ -4225,10 +4240,10 @@
         <v>212</v>
       </c>
       <c r="V2" s="2">
-        <v>43.638491000000002</v>
+        <v>43.636996983501398</v>
       </c>
       <c r="W2" s="2">
-        <v>-79.535400999999993</v>
+        <v>-79.536317735910401</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>1</v>
@@ -4242,16 +4257,16 @@
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>164</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>42</v>
@@ -4287,10 +4302,10 @@
         <v>215</v>
       </c>
       <c r="V3" s="2">
-        <v>43.645274999999998</v>
+        <v>43.645445884617303</v>
       </c>
       <c r="W3" s="2">
-        <v>-79.523955999999998</v>
+        <v>-79.523978568613501</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -4301,16 +4316,16 @@
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>70</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>42</v>
@@ -4346,10 +4361,10 @@
         <v>42</v>
       </c>
       <c r="V4" s="2">
-        <v>43.648271000000001</v>
+        <v>43.648270331180903</v>
       </c>
       <c r="W4" s="2">
-        <v>-79.511062999999993</v>
+        <v>-79.511315524578094</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="105" x14ac:dyDescent="0.25">
@@ -4360,16 +4375,16 @@
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>124</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>42</v>
@@ -4405,10 +4420,10 @@
         <v>42</v>
       </c>
       <c r="V5" s="2">
-        <v>43.650185</v>
+        <v>43.650098799592698</v>
       </c>
       <c r="W5" s="2">
-        <v>-79.495002999999997</v>
+        <v>-79.494966454803901</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -4419,16 +4434,16 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>287</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>37</v>
@@ -4464,10 +4479,10 @@
         <v>42</v>
       </c>
       <c r="V6" s="2">
-        <v>43.649926999999998</v>
+        <v>43.649944993992001</v>
       </c>
       <c r="W6" s="2">
-        <v>-79.483807999999996</v>
+        <v>-79.483824223279896</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="105" x14ac:dyDescent="0.25">
@@ -4478,16 +4493,16 @@
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>291</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>42</v>
@@ -4523,10 +4538,10 @@
         <v>42</v>
       </c>
       <c r="V7" s="2">
-        <v>43.651831999999999</v>
+        <v>43.651695783049703</v>
       </c>
       <c r="W7" s="2">
-        <v>-79.475542000000004</v>
+        <v>-79.475972391664897</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="105" x14ac:dyDescent="0.25">
@@ -4537,13 +4552,13 @@
         <v>7</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>133</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>178</v>
@@ -4582,10 +4597,10 @@
         <v>42</v>
       </c>
       <c r="V8" s="2">
-        <v>43.653955000000003</v>
+        <v>43.653856967991601</v>
       </c>
       <c r="W8" s="2">
-        <v>-79.466498000000001</v>
+        <v>-79.466784149408298</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="105" x14ac:dyDescent="0.25">
@@ -4596,13 +4611,13 @@
         <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>137</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>174</v>
@@ -4641,30 +4656,30 @@
         <v>222</v>
       </c>
       <c r="V9" s="2">
-        <v>43.655462</v>
+        <v>43.655516435484103</v>
       </c>
       <c r="W9" s="2">
-        <v>-79.459577999999993</v>
+        <v>-79.459795318543897</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>135</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>37</v>
@@ -4700,10 +4715,10 @@
         <v>42</v>
       </c>
       <c r="V10" s="2">
-        <v>43.656782</v>
+        <v>43.656971858188598</v>
       </c>
       <c r="W10" s="2">
-        <v>-79.453526999999994</v>
+        <v>-79.452893994748493</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -4714,13 +4729,13 @@
         <v>10</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>131</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>52</v>
@@ -4759,10 +4774,10 @@
         <v>42</v>
       </c>
       <c r="V11" s="2">
-        <v>43.659148999999999</v>
+        <v>43.659249281359997</v>
       </c>
       <c r="W11" s="2">
-        <v>-79.443177000000006</v>
+        <v>-79.442145712673593</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -4773,13 +4788,13 @@
         <v>11</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>143</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>57</v>
@@ -4812,16 +4827,16 @@
         <v>65</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="U12" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V12" s="2">
-        <v>43.660162999999997</v>
+        <v>43.660185549140202</v>
       </c>
       <c r="W12" s="2">
-        <v>-79.435674000000006</v>
+        <v>-79.435454607009802</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -4832,16 +4847,16 @@
         <v>12</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>305</v>
+        <v>333</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>42</v>
@@ -4871,13 +4886,13 @@
         <v>65</v>
       </c>
       <c r="U13" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="V13" s="2">
-        <v>43.662436999999997</v>
+        <v>43.662229278812802</v>
       </c>
       <c r="W13" s="2">
-        <v>-79.426175999999998</v>
+        <v>-79.427018053829599</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -4888,16 +4903,16 @@
         <v>13</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>42</v>
@@ -4927,16 +4942,16 @@
         <v>65</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="U14" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V14" s="2">
-        <v>43.664126000000003</v>
+        <v>43.664116501691801</v>
       </c>
       <c r="W14" s="2">
-        <v>-79.418548999999999</v>
+        <v>-79.418314285576301</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="60" x14ac:dyDescent="0.25">
@@ -4947,16 +4962,16 @@
         <v>14</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>37</v>
@@ -4986,16 +5001,16 @@
         <v>65</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="U15" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V15" s="2">
-        <v>43.666060999999999</v>
+        <v>43.666442887319299</v>
       </c>
       <c r="W15" s="2">
-        <v>-79.411064999999994</v>
+        <v>-79.411212466657105</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="150" x14ac:dyDescent="0.25">
@@ -5005,17 +5020,29 @@
       <c r="B16" s="2">
         <v>15</v>
       </c>
+      <c r="C16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="G16" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>74</v>
@@ -5058,23 +5085,35 @@
       </c>
     </row>
     <row r="17" spans="1:23" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>227</v>
+      <c r="A17" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G17" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>37</v>
@@ -5110,10 +5149,10 @@
         <v>42</v>
       </c>
       <c r="V17" s="2">
-        <v>43.668678999999997</v>
+        <v>43.668263526774602</v>
       </c>
       <c r="W17" s="2">
-        <v>-79.397909999999996</v>
+        <v>-79.399852640926795</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="90" x14ac:dyDescent="0.25">
@@ -5124,16 +5163,16 @@
         <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>42</v>
@@ -5163,36 +5202,48 @@
         <v>211</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="U18" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V18" s="2">
-        <v>43.670136999999997</v>
+        <v>43.670147164753601</v>
       </c>
       <c r="W18" s="2">
-        <v>-79.390709999999999</v>
+        <v>-79.390688538551302</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="135" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>228</v>
+      <c r="A19" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="B19" s="2">
         <v>18</v>
       </c>
+      <c r="C19" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="G19" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>37</v>
@@ -5228,10 +5279,10 @@
         <v>42</v>
       </c>
       <c r="V19" s="2">
-        <v>43.670214999999999</v>
+        <v>43.670934603459003</v>
       </c>
       <c r="W19" s="2">
-        <v>-79.386628000000002</v>
+        <v>-79.385901130735803</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="90" x14ac:dyDescent="0.25">
@@ -5242,16 +5293,16 @@
         <v>19</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>42</v>
@@ -5281,16 +5332,16 @@
         <v>65</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="U20" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V20" s="2">
-        <v>43.672100999999998</v>
+        <v>43.672161454571402</v>
       </c>
       <c r="W20" s="2">
-        <v>-79.376130000000003</v>
+        <v>-79.376247189938994</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="105" x14ac:dyDescent="0.25">
@@ -5301,16 +5352,16 @@
         <v>20</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>42</v>
@@ -5340,36 +5391,36 @@
         <v>65</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="U21" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V21" s="2">
-        <v>43.673605000000002</v>
+        <v>43.673808776185503</v>
       </c>
       <c r="W21" s="2">
-        <v>-79.368819000000002</v>
+        <v>-79.368555955588803</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B22" s="2">
         <v>21</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>37</v>
@@ -5399,16 +5450,16 @@
         <v>65</v>
       </c>
       <c r="T22" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="U22" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V22" s="2">
-        <v>43.676977000000001</v>
+        <v>43.676871951505703</v>
       </c>
       <c r="W22" s="2">
-        <v>-79.358243000000002</v>
+        <v>-79.358313940465393</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -5419,16 +5470,16 @@
         <v>22</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>42</v>
@@ -5458,36 +5509,36 @@
         <v>65</v>
       </c>
       <c r="T23" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="U23" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V23" s="2">
-        <v>43.678227999999997</v>
+        <v>43.6782322887574</v>
       </c>
       <c r="W23" s="2">
-        <v>-79.352452</v>
+        <v>-79.352452307939501</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B24" s="2">
         <v>23</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>37</v>
@@ -5517,16 +5568,16 @@
         <v>65</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="U24" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V24" s="2">
-        <v>43.679924999999997</v>
+        <v>43.679916299905997</v>
       </c>
       <c r="W24" s="2">
-        <v>-79.344556999999995</v>
+        <v>-79.344909265637298</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="105" x14ac:dyDescent="0.25">
@@ -5537,16 +5588,16 @@
         <v>24</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>42</v>
@@ -5576,16 +5627,16 @@
         <v>65</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="U25" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V25" s="2">
-        <v>43.680892</v>
+        <v>43.680980754854602</v>
       </c>
       <c r="W25" s="2">
-        <v>-79.337744999999998</v>
+        <v>-79.337863437831402</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="105" x14ac:dyDescent="0.25">
@@ -5596,16 +5647,16 @@
         <v>25</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>42</v>
@@ -5635,16 +5686,16 @@
         <v>65</v>
       </c>
       <c r="T26" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="U26" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V26" s="2">
-        <v>43.682535000000001</v>
+        <v>43.682576916939702</v>
       </c>
       <c r="W26" s="2">
-        <v>-79.330371</v>
+        <v>-79.330269433557902</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -5655,16 +5706,16 @@
         <v>26</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>42</v>
@@ -5694,16 +5745,16 @@
         <v>65</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="U27" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V27" s="2">
-        <v>43.684078999999997</v>
+        <v>43.684140304773699</v>
       </c>
       <c r="W27" s="2">
-        <v>-79.322918999999999</v>
+        <v>-79.323038868606005</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -5714,16 +5765,16 @@
         <v>27</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>42</v>
@@ -5753,36 +5804,36 @@
         <v>65</v>
       </c>
       <c r="T28" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="U28" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V28" s="2">
-        <v>43.686422</v>
+        <v>43.686406271949899</v>
       </c>
       <c r="W28" s="2">
-        <v>-79.312231999999995</v>
+        <v>-79.312630221247602</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B29" s="2">
         <v>28</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>37</v>
@@ -5812,36 +5863,36 @@
         <v>65</v>
       </c>
       <c r="T29" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="U29" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V29" s="2">
-        <v>43.688861000000003</v>
+        <v>43.689020537960602</v>
       </c>
       <c r="W29" s="2">
-        <v>-79.301804000000004</v>
+        <v>-79.301687143742996</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B30" s="2">
         <v>29</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>37</v>
@@ -5871,16 +5922,16 @@
         <v>65</v>
       </c>
       <c r="T30" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="U30" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="V30" s="2">
-        <v>43.694043999999998</v>
+        <v>43.6946390180591</v>
       </c>
       <c r="W30" s="2">
-        <v>-79.288595999999998</v>
+        <v>-79.289051592350006</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="90" x14ac:dyDescent="0.25">
@@ -5891,16 +5942,16 @@
         <v>30</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>42</v>
@@ -5930,16 +5981,16 @@
         <v>211</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="U31" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="V31" s="2">
-        <v>43.710965000000002</v>
+        <v>43.711441376670699</v>
       </c>
       <c r="W31" s="2">
-        <v>-79.279905999999997</v>
+        <v>-79.279056675732093</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="165" x14ac:dyDescent="0.25">
@@ -5950,16 +6001,16 @@
         <v>31</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>37</v>
@@ -5989,16 +6040,16 @@
         <v>211</v>
       </c>
       <c r="T32" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="U32" s="11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="V32" s="2">
-        <v>43.732269000000002</v>
+        <v>43.732520435051498</v>
       </c>
       <c r="W32" s="2">
-        <v>-79.264010999999996</v>
+        <v>-79.263648055493803</v>
       </c>
     </row>
   </sheetData>
@@ -6012,10 +6063,10 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6040,84 +6091,84 @@
     <col min="19" max="19" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="35.140625" style="11" customWidth="1"/>
     <col min="21" max="21" width="29.42578125" style="12" customWidth="1"/>
-    <col min="22" max="22" width="16.28515625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="64" style="2" customWidth="1"/>
     <col min="25" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="H1" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="I1" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="J1" s="13" t="s">
         <v>414</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>416</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="P1" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>421</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="T1" s="17" t="s">
         <v>424</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="U1" s="17" t="s">
         <v>425</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="W1" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>427</v>
-      </c>
-      <c r="T1" s="17" t="s">
-        <v>428</v>
-      </c>
-      <c r="U1" s="17" t="s">
-        <v>429</v>
-      </c>
-      <c r="V1" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="195" x14ac:dyDescent="0.25">
@@ -6128,16 +6179,16 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>37</v>
@@ -6167,16 +6218,16 @@
         <v>65</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="U2" s="11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="V2" s="2">
-        <v>43.732269000000002</v>
+        <v>43.732520435051498</v>
       </c>
       <c r="W2" s="2">
-        <v>-79.264010999999996</v>
+        <v>-79.263648055493803</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>2</v>
@@ -6184,22 +6235,22 @@
     </row>
     <row r="3" spans="1:24" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>42</v>
@@ -6229,36 +6280,36 @@
         <v>65</v>
       </c>
       <c r="T3" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="U3" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="V3" s="2">
-        <v>43.750492999999999</v>
+        <v>43.750525797094397</v>
       </c>
       <c r="W3" s="2">
-        <v>-79.270285000000001</v>
+        <v>-79.2703016102314</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>42</v>
@@ -6288,36 +6339,36 @@
         <v>65</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="V4" s="2">
-        <v>43.76688</v>
+        <v>43.7669231540699</v>
       </c>
       <c r="W4" s="2">
-        <v>-79.276306000000005</v>
+        <v>-79.276319146156297</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>42</v>
@@ -6347,36 +6398,36 @@
         <v>65</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="U5" s="12" t="s">
         <v>42</v>
       </c>
       <c r="V5" s="2">
-        <v>43.770400000000002</v>
+        <v>43.770401390534801</v>
       </c>
       <c r="W5" s="2">
-        <v>-79.272178999999994</v>
+        <v>-79.272258281707707</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>37</v>
@@ -6406,30 +6457,30 @@
         <v>65</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="U6" s="12" t="s">
         <v>42</v>
       </c>
       <c r="V6" s="2">
-        <v>43.774299999999997</v>
+        <v>43.7743926633839</v>
       </c>
       <c r="W6" s="2">
-        <v>-79.258195000000001</v>
+        <v>-79.258052967488695</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>42</v>
@@ -6459,16 +6510,16 @@
         <v>65</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="U7" s="12" t="s">
         <v>42</v>
       </c>
       <c r="V7" s="2">
-        <v>43.774923999999999</v>
+        <v>43.7749279278692</v>
       </c>
       <c r="W7" s="2">
-        <v>-79.251653000000005</v>
+        <v>-79.251818507909704</v>
       </c>
     </row>
   </sheetData>
@@ -6480,11 +6531,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6515,81 +6566,81 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="H1" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="I1" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="J1" s="13" t="s">
         <v>414</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>416</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="P1" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>421</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="T1" s="17" t="s">
         <v>424</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="U1" s="17" t="s">
         <v>425</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="W1" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="T1" s="17" t="s">
-        <v>428</v>
-      </c>
-      <c r="U1" s="17" t="s">
-        <v>429</v>
-      </c>
-      <c r="V1" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>431</v>
-      </c>
     </row>
     <row r="2" spans="1:24" ht="135" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>267</v>
+      <c r="A2" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -6607,10 +6658,10 @@
         <v>184</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>37</v>
@@ -6646,10 +6697,10 @@
         <v>42</v>
       </c>
       <c r="V2" s="2">
-        <v>43.761564</v>
+        <v>43.762033524372697</v>
       </c>
       <c r="W2" s="2">
-        <v>-79.412107000000006</v>
+        <v>-79.411892406642394</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>3</v>
@@ -6657,22 +6708,22 @@
     </row>
     <row r="3" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>37</v>
@@ -6702,36 +6753,36 @@
         <v>211</v>
       </c>
       <c r="T3" s="11" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="U3" s="12" t="s">
         <v>42</v>
       </c>
       <c r="V3" s="2">
-        <v>43.766841999999997</v>
+        <v>43.766868676392299</v>
       </c>
       <c r="W3" s="2">
-        <v>-79.386277000000007</v>
+        <v>-79.386303797364207</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>37</v>
@@ -6761,36 +6812,36 @@
         <v>211</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="U4" s="12" t="s">
         <v>42</v>
       </c>
       <c r="V4" s="2">
-        <v>43.769055999999999</v>
+        <v>43.769071471991801</v>
       </c>
       <c r="W4" s="2">
-        <v>-79.375916000000004</v>
+        <v>-79.375902526080594</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>37</v>
@@ -6820,30 +6871,30 @@
         <v>211</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="V5" s="2">
-        <v>43.770409999999998</v>
+        <v>43.7710461228518</v>
       </c>
       <c r="W5" s="2">
-        <v>-79.367643999999999</v>
+        <v>-79.366065189242306</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>37</v>
@@ -6873,16 +6924,16 @@
         <v>211</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="V6" s="2">
-        <v>43.775593000000001</v>
+        <v>43.775447935996603</v>
       </c>
       <c r="W6" s="2">
-        <v>-79.346276000000003</v>
+        <v>-79.345614351332102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>